<commit_message>
adapted statistical testing of UK data
</commit_message>
<xml_diff>
--- a/09_Literature_Review/00_Literature Review_Blockchain_Implications for Business Models.xlsx
+++ b/09_Literature_Review/00_Literature Review_Blockchain_Implications for Business Models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/Library/Mobile Documents/3L68KQB4HG~com~readdle~CommonDocuments/Documents/01_Uni/5. Semester/01_Masterarbeit/03_R_Project_MA/09_Literature_Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FAF6D2-001A-A44A-932D-685F615F065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E1F2BF-B996-A840-8BCD-15C61C963D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="I. Design" sheetId="31" r:id="rId1"/>
@@ -4313,7 +4313,7 @@
   </sheetPr>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="111" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="111" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -4824,8 +4824,8 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6312,7 +6312,7 @@
   </sheetPr>
   <dimension ref="B2:AD20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>